<commit_message>
update to files, ref
</commit_message>
<xml_diff>
--- a/working/etterson/seed.fruit.A.xlsx
+++ b/working/etterson/seed.fruit.A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorjaelliott/Desktop/Repositories/LCAdata/working/etterson/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E08274C-3E47-E440-9386-315B81360044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACADEB3-59A0-C74E-81AA-7EA5656F7619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="1360" windowWidth="26440" windowHeight="15440" xr2:uid="{A59A204E-6962-D644-AE36-D5B6E4A58B9F}"/>
+    <workbookView xWindow="8800" yWindow="920" windowWidth="26440" windowHeight="15440" xr2:uid="{A59A204E-6962-D644-AE36-D5B6E4A58B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,6 +473,9 @@
       <c r="C2">
         <v>0.41221374045801529</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -484,6 +487,9 @@
       <c r="C3">
         <v>0.3206106870229008</v>
       </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -495,6 +501,9 @@
       <c r="C4">
         <v>0.41221374045801529</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -506,6 +515,9 @@
       <c r="C5">
         <v>0.37786259541984729</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -517,6 +529,9 @@
       <c r="C6">
         <v>0.30916030534351147</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -528,6 +543,9 @@
       <c r="C7">
         <v>0.27480916030534347</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -539,6 +557,9 @@
       <c r="C8">
         <v>0.29770992366412213</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -549,6 +570,9 @@
       </c>
       <c r="C9">
         <v>0.36641221374045796</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>